<commit_message>
Finished assignment 1 part 1
</commit_message>
<xml_diff>
--- a/מטלה 3/sched.xlsx
+++ b/מטלה 3/sched.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10410"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnpierrehaddad/Desktop/Software_engineering_new/מטלה 3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E9E1BAA1-0384-4FB3-95DC-B9125EC7F334}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{121E5EE4-BCA0-004C-9D78-63790738373E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="68">
   <si>
     <t>Project Planner</t>
   </si>
@@ -159,17 +159,167 @@
     <t>RESPONSIBILITY</t>
   </si>
   <si>
-    <t>Yossi</t>
-  </si>
-  <si>
-    <t>Class A code</t>
+    <t>Class Cart entity code</t>
+  </si>
+  <si>
+    <t>Class Branch entity code</t>
+  </si>
+  <si>
+    <t>Class Client entity code</t>
+  </si>
+  <si>
+    <t>Class Complain entity code</t>
+  </si>
+  <si>
+    <t>Class User entity code</t>
+  </si>
+  <si>
+    <t>Class Branch managerentity code</t>
+  </si>
+  <si>
+    <t>Class Corporation manager entity code</t>
+  </si>
+  <si>
+    <t>Class Item entity code</t>
+  </si>
+  <si>
+    <t>Class Catalog entity code</t>
+  </si>
+  <si>
+    <t>Class Report entity code</t>
+  </si>
+  <si>
+    <t>Class Order Report entity code</t>
+  </si>
+  <si>
+    <t>Class Income Report entity code</t>
+  </si>
+  <si>
+    <t>Class Complain Report entity code</t>
+  </si>
+  <si>
+    <t>John Pierre</t>
+  </si>
+  <si>
+    <t>Lilian</t>
+  </si>
+  <si>
+    <t>Shadi</t>
+  </si>
+  <si>
+    <t>Nour</t>
+  </si>
+  <si>
+    <t>Design SysManager GUI</t>
+  </si>
+  <si>
+    <t>Design Worker GUI</t>
+  </si>
+  <si>
+    <t>Design ServiceW GUI</t>
+  </si>
+  <si>
+    <t>Design BranchManager GUI</t>
+  </si>
+  <si>
+    <t>Design ClientAccount GUI</t>
+  </si>
+  <si>
+    <t>Design ShipPay GUI</t>
+  </si>
+  <si>
+    <t>Design Cart GUI</t>
+  </si>
+  <si>
+    <t>Design ItemShowCatalog GUI</t>
+  </si>
+  <si>
+    <t>Design ItemUpdate GUI</t>
+  </si>
+  <si>
+    <t>Design ItemCart GUI</t>
+  </si>
+  <si>
+    <t>Design ItemCatalog GUI</t>
+  </si>
+  <si>
+    <t>Design Complain GUI</t>
+  </si>
+  <si>
+    <t>Design Catalog GUI</t>
+  </si>
+  <si>
+    <t>Design Report GUI</t>
+  </si>
+  <si>
+    <t>Design CorporationManager GUI</t>
+  </si>
+  <si>
+    <t>Coding SysManager Controller</t>
+  </si>
+  <si>
+    <t>Coding Worker Controller</t>
+  </si>
+  <si>
+    <t>Coding ServiceW Controller</t>
+  </si>
+  <si>
+    <t>Coding BranchManager Controller</t>
+  </si>
+  <si>
+    <t>Coding ClientAccount Controller</t>
+  </si>
+  <si>
+    <t>Coding ShipPay Controller</t>
+  </si>
+  <si>
+    <t>Coding Cart Controller</t>
+  </si>
+  <si>
+    <t>Coding ItemShowCatalog Controller</t>
+  </si>
+  <si>
+    <t>Coding ItemUpdate Controller</t>
+  </si>
+  <si>
+    <t>Coding ItemCart Controller</t>
+  </si>
+  <si>
+    <t>Coding ItemCatalog Controller</t>
+  </si>
+  <si>
+    <t>Coding Complain Controller</t>
+  </si>
+  <si>
+    <t>Coding Catalog Controller</t>
+  </si>
+  <si>
+    <t>Coding Report Controller</t>
+  </si>
+  <si>
+    <t>Coding CorporationManager Controller</t>
+  </si>
+  <si>
+    <t>Design SystemLog GUI</t>
+  </si>
+  <si>
+    <t>Coding SystemLog Controller</t>
+  </si>
+  <si>
+    <t>Feedback on every thing</t>
+  </si>
+  <si>
+    <t>Testing and debugging</t>
+  </si>
+  <si>
+    <t>Everyone</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -271,6 +421,13 @@
       <name val="Corbel"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF404040"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="8">
@@ -487,9 +644,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -573,6 +727,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="19">
@@ -596,7 +753,7 @@
     <cellStyle name="Project Headers" xfId="4" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
     <cellStyle name="Title" xfId="8" builtinId="15" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill>
@@ -624,6 +781,119 @@
         </top>
         <vertical/>
         <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </left>
+        <right style="thin">
+          <color theme="9" tint="-0.24994659260841701"/>
+        </right>
+        <bottom style="thin">
+          <color theme="9" tint="0.59996337778862885"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="lightUp">
+          <fgColor theme="7"/>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor auto="1"/>
+          <bgColor theme="7"/>
+        </patternFill>
+      </fill>
+      <border>
+        <bottom style="thin">
+          <color theme="0"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -983,144 +1253,145 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BP30"/>
+  <dimension ref="B1:BP108"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="3" width="15.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="39.1640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="2" customWidth="1"/>
     <col min="4" max="7" width="11.6640625" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6640625" style="4" customWidth="1"/>
-    <col min="9" max="28" width="2.77734375" style="1"/>
+    <col min="9" max="28" width="2.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:68" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="2:68" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.85">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-    </row>
-    <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="24" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+    </row>
+    <row r="2" spans="2:68" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
       <c r="H2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <v>1</v>
       </c>
-      <c r="K2" s="16"/>
-      <c r="L2" s="30" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="31"/>
-      <c r="N2" s="31"/>
-      <c r="O2" s="31"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="17"/>
-      <c r="R2" s="30" t="s">
+      <c r="M2" s="30"/>
+      <c r="N2" s="30"/>
+      <c r="O2" s="30"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="33"/>
-      <c r="T2" s="33"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="18"/>
-      <c r="W2" s="22" t="s">
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="17"/>
+      <c r="W2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="X2" s="23"/>
-      <c r="Y2" s="23"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="19"/>
-      <c r="AB2" s="35" t="s">
+      <c r="X2" s="22"/>
+      <c r="Y2" s="22"/>
+      <c r="Z2" s="33"/>
+      <c r="AA2" s="18"/>
+      <c r="AB2" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="AC2" s="36"/>
-      <c r="AD2" s="36"/>
-      <c r="AE2" s="36"/>
-      <c r="AF2" s="36"/>
-      <c r="AG2" s="36"/>
-      <c r="AH2" s="37"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="22" t="s">
+      <c r="AC2" s="35"/>
+      <c r="AD2" s="35"/>
+      <c r="AE2" s="35"/>
+      <c r="AF2" s="35"/>
+      <c r="AG2" s="35"/>
+      <c r="AH2" s="36"/>
+      <c r="AI2" s="19"/>
+      <c r="AJ2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="AK2" s="23"/>
-      <c r="AL2" s="23"/>
-      <c r="AM2" s="23"/>
-      <c r="AN2" s="23"/>
-      <c r="AO2" s="23"/>
-      <c r="AP2" s="23"/>
-      <c r="AQ2" s="23"/>
-    </row>
-    <row r="3" spans="2:68" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="AK2" s="22"/>
+      <c r="AL2" s="22"/>
+      <c r="AM2" s="22"/>
+      <c r="AN2" s="22"/>
+      <c r="AO2" s="22"/>
+      <c r="AP2" s="22"/>
+      <c r="AQ2" s="22"/>
+    </row>
+    <row r="3" spans="2:68" s="11" customFormat="1" ht="40" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="27" t="s">
+      <c r="G3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="29" t="s">
+      <c r="H3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
-      <c r="AB3" s="11"/>
-    </row>
-    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+      <c r="AA3" s="10"/>
+      <c r="AB3" s="10"/>
+    </row>
+    <row r="4" spans="2:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="25"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
       <c r="I4" s="3">
         <v>1</v>
       </c>
@@ -1302,247 +1573,1274 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="E5" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+    <row r="6" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="7">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
+        <v>6</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="8"/>
     </row>
-    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+    <row r="7" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>6</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="8"/>
     </row>
-    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+    <row r="8" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="8"/>
     </row>
-    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+    <row r="9" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="7">
+        <v>1</v>
+      </c>
+      <c r="E9" s="7">
+        <v>6</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="8"/>
     </row>
-    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+    <row r="10" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1</v>
+      </c>
+      <c r="E10" s="7">
+        <v>6</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="8"/>
     </row>
-    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+    <row r="11" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="7">
+        <v>6</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="8"/>
     </row>
-    <row r="12" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+    <row r="12" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="7">
+        <v>6</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="8"/>
     </row>
-    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+    <row r="13" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <v>6</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="8"/>
     </row>
-    <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+    <row r="14" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <v>6</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="8"/>
     </row>
-    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="7"/>
+    <row r="15" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="7">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <v>6</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="8"/>
     </row>
-    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+    <row r="16" spans="2:68" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="7">
+        <v>1</v>
+      </c>
+      <c r="E16" s="7">
+        <v>6</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="8"/>
     </row>
-    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <v>6</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="8"/>
     </row>
-    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="7">
+        <v>7</v>
+      </c>
+      <c r="E18" s="7">
+        <v>1</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="8"/>
     </row>
-    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="7"/>
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="7">
+        <v>8</v>
+      </c>
+      <c r="E19" s="7">
+        <v>10</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="8"/>
     </row>
-    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="7">
+        <v>8</v>
+      </c>
+      <c r="E20" s="7">
+        <v>10</v>
+      </c>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="8"/>
     </row>
-    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="7">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7">
+        <v>10</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="8"/>
     </row>
-    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="7">
+        <v>8</v>
+      </c>
+      <c r="E22" s="7">
+        <v>10</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="8"/>
     </row>
-    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D23" s="7">
+        <v>8</v>
+      </c>
+      <c r="E23" s="7">
+        <v>10</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="7">
+        <v>8</v>
+      </c>
+      <c r="E24" s="7">
+        <v>10</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="7">
+        <v>8</v>
+      </c>
+      <c r="E25" s="7">
+        <v>10</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
+    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C26" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" s="7">
+        <v>8</v>
+      </c>
+      <c r="E26" s="7">
+        <v>10</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D27" s="7">
+        <v>8</v>
+      </c>
+      <c r="E27" s="7">
+        <v>10</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
+    <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C28" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D28" s="7">
+        <v>8</v>
+      </c>
+      <c r="E28" s="7">
+        <v>10</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
+    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" s="7">
+        <v>8</v>
+      </c>
+      <c r="E29" s="7">
+        <v>10</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
+    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C30" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D30" s="7">
+        <v>8</v>
+      </c>
+      <c r="E30" s="7">
+        <v>10</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="7"/>
       <c r="H30" s="8"/>
+    </row>
+    <row r="31" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D31" s="7">
+        <v>8</v>
+      </c>
+      <c r="E31" s="7">
+        <v>10</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8"/>
+    </row>
+    <row r="32" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D32" s="7">
+        <v>8</v>
+      </c>
+      <c r="E32" s="7">
+        <v>10</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+    </row>
+    <row r="33" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C33" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D33" s="7">
+        <v>8</v>
+      </c>
+      <c r="E33" s="7">
+        <v>10</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="8"/>
+    </row>
+    <row r="34" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" s="7">
+        <v>8</v>
+      </c>
+      <c r="E34" s="7">
+        <v>10</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D35" s="7">
+        <v>18</v>
+      </c>
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="7">
+        <v>19</v>
+      </c>
+      <c r="E36" s="7">
+        <v>16</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="8"/>
+    </row>
+    <row r="37" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C37" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="7">
+        <v>19</v>
+      </c>
+      <c r="E37" s="7">
+        <v>16</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="8"/>
+    </row>
+    <row r="38" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C38" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="7">
+        <v>19</v>
+      </c>
+      <c r="E38" s="7">
+        <v>16</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="39" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="7">
+        <v>19</v>
+      </c>
+      <c r="E39" s="7">
+        <v>16</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8"/>
+    </row>
+    <row r="40" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D40" s="7">
+        <v>19</v>
+      </c>
+      <c r="E40" s="7">
+        <v>16</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="8"/>
+    </row>
+    <row r="41" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D41" s="7">
+        <v>19</v>
+      </c>
+      <c r="E41" s="7">
+        <v>16</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8"/>
+    </row>
+    <row r="42" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C42" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D42" s="7">
+        <v>19</v>
+      </c>
+      <c r="E42" s="7">
+        <v>16</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8"/>
+    </row>
+    <row r="43" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D43" s="7">
+        <v>19</v>
+      </c>
+      <c r="E43" s="7">
+        <v>16</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="8"/>
+    </row>
+    <row r="44" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D44" s="7">
+        <v>19</v>
+      </c>
+      <c r="E44" s="7">
+        <v>16</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8"/>
+    </row>
+    <row r="45" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C45" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="7">
+        <v>19</v>
+      </c>
+      <c r="E45" s="7">
+        <v>16</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="8"/>
+    </row>
+    <row r="46" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="7">
+        <v>19</v>
+      </c>
+      <c r="E46" s="7">
+        <v>16</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="8"/>
+    </row>
+    <row r="47" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="7">
+        <v>19</v>
+      </c>
+      <c r="E47" s="7">
+        <v>16</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8"/>
+    </row>
+    <row r="48" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="7">
+        <v>19</v>
+      </c>
+      <c r="E48" s="7">
+        <v>16</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="8"/>
+    </row>
+    <row r="49" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="D49" s="7">
+        <v>19</v>
+      </c>
+      <c r="E49" s="7">
+        <v>16</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="8"/>
+    </row>
+    <row r="50" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" s="7">
+        <v>19</v>
+      </c>
+      <c r="E50" s="7">
+        <v>16</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8"/>
+    </row>
+    <row r="51" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B51" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C51" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="D51" s="7">
+        <v>19</v>
+      </c>
+      <c r="E51" s="7">
+        <v>16</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="7"/>
+      <c r="H51" s="8"/>
+    </row>
+    <row r="52" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
+      <c r="F52" s="7"/>
+      <c r="G52" s="7"/>
+      <c r="H52" s="8"/>
+    </row>
+    <row r="53" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="7">
+        <v>35</v>
+      </c>
+      <c r="E53" s="7">
+        <v>10</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="7"/>
+      <c r="H53" s="8"/>
+    </row>
+    <row r="54" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C54" s="6"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
+      <c r="F54" s="7"/>
+      <c r="G54" s="7"/>
+      <c r="H54" s="8"/>
+    </row>
+    <row r="55" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C55" s="6"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7"/>
+      <c r="G55" s="7"/>
+      <c r="H55" s="8"/>
+    </row>
+    <row r="56" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C56" s="6"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+      <c r="F56" s="7"/>
+      <c r="G56" s="7"/>
+      <c r="H56" s="8"/>
+    </row>
+    <row r="57" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C57" s="6"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+      <c r="G57" s="7"/>
+      <c r="H57" s="8"/>
+    </row>
+    <row r="58" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C58" s="6"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
+      <c r="H58" s="8"/>
+    </row>
+    <row r="59" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C59" s="6"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
+      <c r="H59" s="8"/>
+    </row>
+    <row r="60" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C60" s="6"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
+      <c r="H60" s="8"/>
+    </row>
+    <row r="61" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C61" s="6"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7"/>
+      <c r="G61" s="7"/>
+      <c r="H61" s="8"/>
+    </row>
+    <row r="62" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C62" s="6"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="8"/>
+    </row>
+    <row r="63" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C63" s="6"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7"/>
+      <c r="G63" s="7"/>
+      <c r="H63" s="8"/>
+    </row>
+    <row r="64" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C64" s="6"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+      <c r="F64" s="7"/>
+      <c r="G64" s="7"/>
+      <c r="H64" s="8"/>
+    </row>
+    <row r="65" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C65" s="6"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7"/>
+      <c r="G65" s="7"/>
+      <c r="H65" s="8"/>
+    </row>
+    <row r="66" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C66" s="6"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+      <c r="G66" s="7"/>
+      <c r="H66" s="8"/>
+    </row>
+    <row r="67" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C67" s="6"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="8"/>
+    </row>
+    <row r="68" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C68" s="6"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="8"/>
+    </row>
+    <row r="69" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C69" s="6"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="8"/>
+    </row>
+    <row r="70" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C70" s="6"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="8"/>
+    </row>
+    <row r="71" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C71" s="6"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="8"/>
+    </row>
+    <row r="72" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C72" s="6"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="8"/>
+    </row>
+    <row r="73" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C73" s="6"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7"/>
+      <c r="H73" s="8"/>
+    </row>
+    <row r="74" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C74" s="6"/>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7"/>
+      <c r="G74" s="7"/>
+      <c r="H74" s="8"/>
+    </row>
+    <row r="75" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C75" s="6"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7"/>
+      <c r="H75" s="8"/>
+    </row>
+    <row r="76" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C76" s="6"/>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+      <c r="G76" s="7"/>
+      <c r="H76" s="8"/>
+    </row>
+    <row r="77" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C77" s="6"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7"/>
+      <c r="H77" s="8"/>
+    </row>
+    <row r="78" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C78" s="6"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+      <c r="F78" s="7"/>
+      <c r="G78" s="7"/>
+      <c r="H78" s="8"/>
+    </row>
+    <row r="79" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C79" s="6"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7"/>
+      <c r="H79" s="8"/>
+    </row>
+    <row r="80" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C80" s="6"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+      <c r="F80" s="7"/>
+      <c r="G80" s="7"/>
+      <c r="H80" s="8"/>
+    </row>
+    <row r="81" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C81" s="6"/>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="8"/>
+    </row>
+    <row r="82" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C82" s="6"/>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+      <c r="F82" s="7"/>
+      <c r="G82" s="7"/>
+      <c r="H82" s="8"/>
+    </row>
+    <row r="83" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C83" s="6"/>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7"/>
+      <c r="G83" s="7"/>
+      <c r="H83" s="8"/>
+    </row>
+    <row r="84" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C84" s="6"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="7"/>
+      <c r="H84" s="8"/>
+    </row>
+    <row r="85" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C85" s="6"/>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7"/>
+      <c r="G85" s="7"/>
+      <c r="H85" s="8"/>
+    </row>
+    <row r="86" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C86" s="6"/>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+      <c r="F86" s="7"/>
+      <c r="G86" s="7"/>
+      <c r="H86" s="8"/>
+    </row>
+    <row r="87" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C87" s="6"/>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+      <c r="G87" s="7"/>
+      <c r="H87" s="8"/>
+    </row>
+    <row r="88" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C88" s="6"/>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+      <c r="F88" s="7"/>
+      <c r="G88" s="7"/>
+      <c r="H88" s="8"/>
+    </row>
+    <row r="89" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C89" s="6"/>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+      <c r="F89" s="7"/>
+      <c r="G89" s="7"/>
+      <c r="H89" s="8"/>
+    </row>
+    <row r="90" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C90" s="6"/>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+      <c r="G90" s="7"/>
+      <c r="H90" s="8"/>
+    </row>
+    <row r="91" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C91" s="6"/>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7"/>
+      <c r="G91" s="7"/>
+      <c r="H91" s="8"/>
+    </row>
+    <row r="92" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C92" s="6"/>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+      <c r="F92" s="7"/>
+      <c r="G92" s="7"/>
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C93" s="6"/>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+      <c r="F93" s="7"/>
+      <c r="G93" s="7"/>
+      <c r="H93" s="8"/>
+    </row>
+    <row r="94" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C94" s="6"/>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+      <c r="F94" s="7"/>
+      <c r="G94" s="7"/>
+      <c r="H94" s="8"/>
+    </row>
+    <row r="95" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C95" s="6"/>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+      <c r="F95" s="7"/>
+      <c r="G95" s="7"/>
+      <c r="H95" s="8"/>
+    </row>
+    <row r="96" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C96" s="6"/>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+      <c r="F96" s="7"/>
+      <c r="G96" s="7"/>
+      <c r="H96" s="8"/>
+    </row>
+    <row r="97" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C97" s="6"/>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+      <c r="F97" s="7"/>
+      <c r="G97" s="7"/>
+      <c r="H97" s="8"/>
+    </row>
+    <row r="98" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C98" s="6"/>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="7"/>
+      <c r="H98" s="8"/>
+    </row>
+    <row r="99" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C99" s="6"/>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+      <c r="F99" s="7"/>
+      <c r="G99" s="7"/>
+      <c r="H99" s="8"/>
+    </row>
+    <row r="100" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C100" s="6"/>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+      <c r="F100" s="7"/>
+      <c r="G100" s="7"/>
+      <c r="H100" s="8"/>
+    </row>
+    <row r="101" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C101" s="6"/>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7"/>
+      <c r="G101" s="7"/>
+      <c r="H101" s="8"/>
+    </row>
+    <row r="102" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C102" s="6"/>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7"/>
+      <c r="G102" s="7"/>
+      <c r="H102" s="8"/>
+    </row>
+    <row r="103" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C103" s="6"/>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7"/>
+      <c r="G103" s="7"/>
+      <c r="H103" s="8"/>
+    </row>
+    <row r="104" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C104" s="6"/>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+      <c r="F104" s="7"/>
+      <c r="G104" s="7"/>
+      <c r="H104" s="8"/>
+    </row>
+    <row r="105" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C105" s="6"/>
+      <c r="D105" s="7"/>
+      <c r="E105" s="7"/>
+      <c r="F105" s="7"/>
+      <c r="G105" s="7"/>
+      <c r="H105" s="8"/>
+    </row>
+    <row r="106" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C106" s="6"/>
+      <c r="D106" s="7"/>
+      <c r="E106" s="7"/>
+      <c r="F106" s="7"/>
+      <c r="G106" s="7"/>
+      <c r="H106" s="8"/>
+    </row>
+    <row r="107" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C107" s="6"/>
+      <c r="D107" s="7"/>
+      <c r="E107" s="7"/>
+      <c r="F107" s="7"/>
+      <c r="G107" s="7"/>
+      <c r="H107" s="8"/>
+    </row>
+    <row r="108" spans="3:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C108" s="6"/>
+      <c r="D108" s="7"/>
+      <c r="E108" s="7"/>
+      <c r="F108" s="7"/>
+      <c r="G108" s="7"/>
+      <c r="H108" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -1560,7 +2858,7 @@
     <mergeCell ref="AB2:AH2"/>
     <mergeCell ref="C3:C4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I5:BP30">
+  <conditionalFormatting sqref="I5:BP108">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1586,17 +2884,12 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:BP31">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>TRUE</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="I4:BP4">
     <cfRule type="expression" dxfId="0" priority="8">
       <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="16">
+  <dataValidations count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="I2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>

</xml_diff>